<commit_message>
Sample data to spreadsheet for CRUD operations
</commit_message>
<xml_diff>
--- a/modA/spreadsheet.xlsx
+++ b/modA/spreadsheet.xlsx
@@ -11,19 +11,141 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+  <si>
+    <t>Date Time</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>Connor</t>
+  </si>
+  <si>
+    <t>Pencil</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>Shane</t>
+  </si>
+  <si>
+    <t>Binder</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>Thatcher</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>04-23-2014 02:25</t>
+  </si>
+  <si>
+    <t>12-26-2014 09:54</t>
+  </si>
+  <si>
+    <t>03-15-2014 06:00</t>
+  </si>
+  <si>
+    <t>04-18-2014 12:00</t>
+  </si>
+  <si>
+    <t>04-23-2014 02:26</t>
+  </si>
+  <si>
+    <t>12-26-2014 09:55</t>
+  </si>
+  <si>
+    <t>03-15-2014 06:01</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Naga Pavan</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Rajiv</t>
+  </si>
+  <si>
+    <t>Minhaj</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +168,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +473,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>41797.201388888891</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="G2" s="1">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>399.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>41887.197916666664</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="G4" s="1">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>599.70000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="G6" s="1">
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>41643</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="G7" s="1">
+        <v>199.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="G8" s="1">
+        <v>89.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>41798.201388888891</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>399.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29.25">
+      <c r="A11" s="2">
+        <v>41888.197916608799</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="G11" s="1">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G12" s="1">
+        <v>599.70000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="G13" s="1">
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
+        <v>41644</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="G14" s="1">
+        <v>199.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
+        <v>41798.201388888891</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="G15" s="1">
+        <v>89.55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>